<commit_message>
Refactor coverage reporting and clean up test artifacts
- Updated `.gitignore` to include coverage directory for tests.
- Modified `Makefile` to change coverage report output path and clean commands to remove test coverage artifacts.
- Process test emails.
- Enhanced error handling in `localized_app.py` for text analysis with retry mechanism and fallback responses.
- Added localization for error messages in `text_analysis_localization.py`.
</commit_message>
<xml_diff>
--- a/runtime_dev/apps/delphes78/delphes78.xlsx
+++ b/runtime_dev/apps/delphes78/delphes78.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime_dev/apps/delphes78/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18D5E3A-D1E8-E64A-ADD0-EDD8B55E7EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F86DAA-0EA3-4B4A-AF07-17D36EDCA2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="5" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -2105,7 +2105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -2457,7 +2457,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>332</v>
       </c>
@@ -2711,7 +2711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C9" sqref="A3:C9"/>
     </sheetView>
   </sheetViews>
@@ -4957,15 +4957,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F212B83-BB31-486E-8D1E-C153171C389E}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.6640625" customWidth="1"/>
-    <col min="2" max="2" width="90.1640625" customWidth="1"/>
-    <col min="3" max="3" width="108.33203125" customWidth="1"/>
+    <col min="2" max="3" width="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -4990,7 +4989,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -5023,7 +5022,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>

</xml_diff>